<commit_message>
20230112 Pyspark test datset
</commit_message>
<xml_diff>
--- a/Notes/03 Pyspark with Python/test.xlsx
+++ b/Notes/03 Pyspark with Python/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -295,6 +295,15 @@
   </si>
   <si>
     <t>sonal@gmail.com</t>
+  </si>
+  <si>
+    <t>vinod</t>
+  </si>
+  <si>
+    <t>kadam</t>
+  </si>
+  <si>
+    <t>vinod#gmail.com</t>
   </si>
 </sst>
 </file>
@@ -623,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,19 +720,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="C4">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -737,36 +746,36 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>1.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>27</v>
@@ -775,198 +784,198 @@
         <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H6">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H7">
-        <v>2.6</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H8">
-        <v>4.8</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H9">
-        <v>3.5</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
         <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="H10">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H11">
-        <v>4.7</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C12">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H12">
-        <v>4.0999999999999996</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="H13">
-        <v>2.2999999999999998</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -974,7 +983,7 @@
         <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14">
         <v>26</v>
@@ -983,128 +992,128 @@
         <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C15">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="H16">
-        <v>3.1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="H17">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C18">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="H18">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>28</v>
@@ -1113,7 +1122,7 @@
         <v>54</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -1127,131 +1136,157 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C20">
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H20">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
       </c>
       <c r="C21">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="H21">
-        <v>4.0999999999999996</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="H22">
-        <v>2.4</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C23">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
         <v>55</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="H23">
-        <v>3.6</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C24">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
         <v>55</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
         <v>19</v>
       </c>
       <c r="G24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
         <v>20</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>4.3</v>
       </c>
     </row>
@@ -1259,27 +1294,27 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
-    <hyperlink ref="E17" r:id="rId16"/>
-    <hyperlink ref="E18" r:id="rId17"/>
-    <hyperlink ref="E19" r:id="rId18"/>
-    <hyperlink ref="E20" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E22" r:id="rId21"/>
-    <hyperlink ref="E23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E10" r:id="rId8"/>
+    <hyperlink ref="E11" r:id="rId9"/>
+    <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E14" r:id="rId12"/>
+    <hyperlink ref="E15" r:id="rId13"/>
+    <hyperlink ref="E16" r:id="rId14"/>
+    <hyperlink ref="E17" r:id="rId15"/>
+    <hyperlink ref="E18" r:id="rId16"/>
+    <hyperlink ref="E19" r:id="rId17"/>
+    <hyperlink ref="E20" r:id="rId18"/>
+    <hyperlink ref="E21" r:id="rId19"/>
+    <hyperlink ref="E22" r:id="rId20"/>
+    <hyperlink ref="E23" r:id="rId21"/>
+    <hyperlink ref="E24" r:id="rId22"/>
+    <hyperlink ref="E25" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId24"/>

</xml_diff>